<commit_message>
update ts tests to use monthly diffs and rates for 12 lags
</commit_message>
<xml_diff>
--- a/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/A Diff-in-DiffDAGOLS 2010-01-31 to 2020-02-29 orig0.1.xlsx
+++ b/MappingTheFederalReserve'sResponseFunctionWithDirectedAcyclicGraphs/A Diff-in-DiffDAGOLS 2010-01-31 to 2020-02-29 orig0.1.xlsx
@@ -31,16 +31,16 @@
     <t>C Lag</t>
   </si>
   <si>
-    <t>-0.27***</t>
-  </si>
-  <si>
-    <t>-2.821***</t>
-  </si>
-  <si>
-    <t>-0.012*</t>
-  </si>
-  <si>
-    <t>-0.467***</t>
+    <t>-0.372***</t>
+  </si>
+  <si>
+    <t>-3.464***</t>
+  </si>
+  <si>
+    <t>0.01*</t>
+  </si>
+  <si>
+    <t>-0.808***</t>
   </si>
 </sst>
 </file>

</xml_diff>